<commit_message>
Added results for contradiction check of compositions
</commit_message>
<xml_diff>
--- a/results/correct models/R10-file-manager/compositions_contradiction_check.xlsx
+++ b/results/correct models/R10-file-manager/compositions_contradiction_check.xlsx
@@ -1,37 +1,67 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
   <workbookPr/>
-  <workbookProtection/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Thesis\semantic-alignment-detection\results\correct models\R10-file-manager\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A02A8912-5360-45A9-9146-BF733FAC3388}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames/>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+  <si>
+    <t>actual_description</t>
+  </si>
+  <si>
+    <t>generated_description</t>
+  </si>
+  <si>
+    <t>A file system contains information from multiple documents.</t>
+  </si>
+  <si>
+    <t>Each file system is made up of zero or multiple documents</t>
+  </si>
+  <si>
+    <t>llm response</t>
+  </si>
+  <si>
+    <t>Statement 2 says that a file system "contains information from multiple documents". This suggests that a file system uses documents to store its data, as it is able to contain information from these documents. Combined with statement 1 that mentions each file system is made up of zero or multiple documents, it is reasonable to conclude that a document is a part of a file system and a file system is composed of documents.
+Conclusion: Yes</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="0"/>
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b val="1"/>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill/>
+      <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -46,93 +76,46 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <indexedColors>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00000000"/>
-      <rgbColor rgb="00FFFFFF"/>
-      <rgbColor rgb="00FF0000"/>
-      <rgbColor rgb="0000FF00"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008000"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00808000"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="00C0C0C0"/>
-      <rgbColor rgb="00808080"/>
-      <rgbColor rgb="009999FF"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00FFFFCC"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00660066"/>
-      <rgbColor rgb="00FF8080"/>
-      <rgbColor rgb="000066CC"/>
-      <rgbColor rgb="00CCCCFF"/>
-      <rgbColor rgb="00000080"/>
-      <rgbColor rgb="00FF00FF"/>
-      <rgbColor rgb="00FFFF00"/>
-      <rgbColor rgb="0000FFFF"/>
-      <rgbColor rgb="00800080"/>
-      <rgbColor rgb="00800000"/>
-      <rgbColor rgb="00008080"/>
-      <rgbColor rgb="000000FF"/>
-      <rgbColor rgb="0000CCFF"/>
-      <rgbColor rgb="00CCFFFF"/>
-      <rgbColor rgb="00CCFFCC"/>
-      <rgbColor rgb="00FFFF99"/>
-      <rgbColor rgb="0099CCFF"/>
-      <rgbColor rgb="00FF99CC"/>
-      <rgbColor rgb="00CC99FF"/>
-      <rgbColor rgb="00FFCC99"/>
-      <rgbColor rgb="003366FF"/>
-      <rgbColor rgb="0033CCCC"/>
-      <rgbColor rgb="0099CC00"/>
-      <rgbColor rgb="00FFCC00"/>
-      <rgbColor rgb="00FF9900"/>
-      <rgbColor rgb="00FF6600"/>
-      <rgbColor rgb="00666699"/>
-      <rgbColor rgb="00969696"/>
-      <rgbColor rgb="00003366"/>
-      <rgbColor rgb="00339966"/>
-      <rgbColor rgb="00003300"/>
-      <rgbColor rgb="00333300"/>
-      <rgbColor rgb="00993300"/>
-      <rgbColor rgb="00993366"/>
-      <rgbColor rgb="00333399"/>
-      <rgbColor rgb="00333333"/>
-    </indexedColors>
-  </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -420,164 +403,48 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="28.08984375" customWidth="1"/>
+    <col min="2" max="2" width="41.6328125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>actual_description</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>generated_description</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Do these statements contradict each other? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Are these statements mutually exclusive? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Do these statements clash or conflict with each other? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Are these statements at odds with each other? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Do these statements negate each other? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Are these statements inconsistent? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Do these statements oppose each other? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Are these statements in disagreement? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Are these statements incompatible? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Do these statements present conflicting viewpoints? 
- Statement1:{statement1} 
- Statement2:{statement2}</t>
-        </is>
-      </c>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+      <c r="K1" s="1"/>
+      <c r="L1" s="1"/>
     </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>A file system contains information from multiple documents.</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Each file system is made up of zero or multiple documents</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>No, these statements do not contradict each other. Statement 1 says that a file system can have no documents or multiple documents. Statement 2 implies that in a scenario where there are multiple documents, the file system represents or contains information from them.</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>No, these statements are not mutually exclusive. A file system can contain multiple documents as mentioned in both Statement 1 and Statement 2. The second statement implies that there is information drawn from multiple documents in the file system, which fits squarely within the possibility presented in Statement 1 that there can be multiple documents in a file system.</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>These statements do not necessarily clash or conflict with each other, but they can be interpreted in potentially conflicting ways based on how you define a "file system" and a "document."
-In one interpretation, Statement 1 could mean that a file system can exist without documents (given the "zero" quantity), while Statement 2 implies that a file system must always contain multiple documents' information. In this scenario, they would be conflicting.
-However, if you interpret Statement 2 as saying "a file system has the capacity to contain information from multiple documents" (meaning it doesn't always have to), then the statements do not conflict. 
-The conflict arises based on the implied necessity in Statement 2 — whether a file system containing multiple documents' information is an inherent requirement or just a possible condition.</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>No, these statements are not at odds with each other. Though the first statement mentions that a file system can consist of zero documents, it also acknowledges that it can contain multiple documents, which groups it in harmony with the second statement that a file system contains information from multiple documents.</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>No, these statements do not negate each other. The first statement describes the potential number of documents a file system could have, including zero or multiple. The second statement implies that a file system already contains information from more than one document, but it doesn't contradict the first statement because it's possible that some file systems have multiple documents while others do not.</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>No, these statements are not inconsistent. However, the understanding might differ slightly. The first statement implies that a file system might not contain any documents at all, while the second statement suggests that a file system contains information from multiple documents, indicating the presence of at least some documents. To make these two statements perfectly consistent, the second statement could be modified to specify "one or multiple documents" instead of "multiple documents".</t>
-        </is>
-      </c>
-      <c r="I2" t="inlineStr">
-        <is>
-          <t>No, these statements do not oppose each other. The first statement explains that a file system can have multiple documents. The second statement just states one of the things the file system does, which is containing information from these documents.</t>
-        </is>
-      </c>
-      <c r="J2" t="inlineStr">
-        <is>
-          <t>No, these statements are not in disagreement. The first statement says that a file system can contain multiple documents. The second statement implies the same, stating that a file system contains information from multiple documents. However, it's important to note that statement 2 also implicitly suggests that these documents contain information, which is an additional detail not covered in statement 1.</t>
-        </is>
-      </c>
-      <c r="K2" t="inlineStr">
-        <is>
-          <t>No, these statements are not incompatible. However, they might not both be true at the same time. The first statement allows for the possibility that a file system may contain no documents, while the second statement asserts that a file system does contain information from multiple documents. So, while they're not directly contradictory, if a file system has zero documents, then the second statement would not be true for that file system.</t>
-        </is>
-      </c>
-      <c r="L2" t="inlineStr">
-        <is>
-          <t>No, these statements do not present conflicting viewpoints. They both agree that a file system can contain multiple documents. The first statement just adds that it could also contain zero documents.</t>
-        </is>
+    <row r="2" spans="1:12" ht="409.5" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>